<commit_message>
Prepare for release (#445)
* prepare benchmark release

* update results
</commit_message>
<xml_diff>
--- a/benchmark/leaderboard.xlsx
+++ b/benchmark/leaderboard.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/repos-to-trash/Orion/benchmark/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3224E60B-F6C9-3D49-99E8-51EBE1625E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="0.5.0-Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="0.5.0-F1-Scores" sheetId="2" r:id="rId2"/>
+    <sheet name="v0.5.1-Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="v0.5.1-F1-Scores" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>aer</t>
   </si>
@@ -29,18 +23,18 @@
     <t>lstm_dynamic_threshold</t>
   </si>
   <si>
+    <t>lstm_autoencoder</t>
+  </si>
+  <si>
+    <t>vae</t>
+  </si>
+  <si>
+    <t>tadgan</t>
+  </si>
+  <si>
     <t>arima</t>
   </si>
   <si>
-    <t>lstm_autoencoder</t>
-  </si>
-  <si>
-    <t>vae</t>
-  </si>
-  <si>
-    <t>tadgan</t>
-  </si>
-  <si>
     <t>dense_autoencoder</t>
   </si>
   <si>
@@ -72,6 +66,9 @@
   </si>
   <si>
     <t>SMAP</t>
+  </si>
+  <si>
+    <t>UCR</t>
   </si>
   <si>
     <t>YAHOO</t>
@@ -116,8 +113,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,12 +165,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -183,14 +177,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -237,7 +223,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,27 +255,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,24 +289,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -514,21 +464,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -545,24 +495,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
-        <v>1837</v>
+        <v>2231</v>
       </c>
       <c r="D2" s="1">
-        <v>0.74539999999999995</v>
+        <v>0.704</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -570,115 +520,115 @@
         <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>1726</v>
+        <v>2084</v>
       </c>
       <c r="D3" s="1">
-        <v>0.64610000000000001</v>
+        <v>0.6237</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="1">
+        <v>8</v>
+      </c>
       <c r="C4" s="1">
-        <v>1735</v>
+        <v>1641</v>
       </c>
       <c r="D4" s="1">
-        <v>0.57769999999999999</v>
+        <v>0.5537</v>
       </c>
       <c r="E4" s="1">
-        <v>0.11550000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.0003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>1038</v>
+        <v>1655</v>
       </c>
       <c r="D5" s="1">
-        <v>0.57540000000000002</v>
+        <v>0.5465</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.0003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>1192</v>
+        <v>1861</v>
       </c>
       <c r="D6" s="1">
-        <v>0.56559999999999999</v>
+        <v>0.5433</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.0016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>7</v>
-      </c>
       <c r="C7" s="1">
-        <v>1273</v>
+        <v>1930</v>
       </c>
       <c r="D7" s="1">
-        <v>0.54959999999999998</v>
+        <v>0.5372</v>
       </c>
       <c r="E7" s="1">
-        <v>1.6999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.1444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>593</v>
+        <v>984</v>
       </c>
       <c r="D8" s="1">
-        <v>0.53720000000000001</v>
+        <v>0.5007</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>296</v>
+        <v>793</v>
       </c>
       <c r="D9" s="1">
-        <v>0.37680000000000002</v>
+        <v>0.3577</v>
       </c>
       <c r="E9" s="1">
-        <v>3.2300000000000002E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.0296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -686,10 +636,10 @@
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>15232</v>
+        <v>20912</v>
       </c>
       <c r="D10" s="1">
-        <v>0.25080000000000002</v>
+        <v>0.2239</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -701,53 +651,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="21.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
-    <col min="7" max="14" width="21.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
+      <c r="O1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
@@ -755,7 +715,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>19</v>
@@ -767,7 +727,7 @@
         <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>24</v>
@@ -781,413 +741,443 @@
       <c r="L2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>0.63160000000000005</v>
+        <v>0.5753</v>
       </c>
       <c r="C3" s="1">
-        <v>0.78400000000000003</v>
+        <v>0.8031</v>
       </c>
       <c r="D3" s="1">
-        <v>0.76739999999999997</v>
+        <v>0.4824</v>
       </c>
       <c r="E3" s="1">
-        <v>0.97770000000000001</v>
+        <v>0.7988</v>
       </c>
       <c r="F3" s="1">
-        <v>0.87849999999999995</v>
+        <v>0.9875</v>
       </c>
       <c r="G3" s="1">
-        <v>0.70850000000000002</v>
+        <v>0.8977000000000001</v>
       </c>
       <c r="H3" s="1">
-        <v>0.76919999999999999</v>
+        <v>0.7125</v>
       </c>
       <c r="I3" s="1">
-        <v>0.72729999999999995</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="1">
-        <v>0.66669999999999996</v>
+        <v>0.75</v>
       </c>
       <c r="K3" s="1">
-        <v>0.68569999999999998</v>
+        <v>0.6667</v>
       </c>
       <c r="L3" s="1">
-        <v>0.60319999999999996</v>
+        <v>0.7027</v>
       </c>
       <c r="M3" s="1">
-        <v>0.74539999999999995</v>
+        <v>0.5714</v>
       </c>
       <c r="N3" s="1">
-        <v>0.10390000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.704</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.1486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>0.43480000000000002</v>
+        <v>0.4348</v>
       </c>
       <c r="C4" s="1">
-        <v>0.32390000000000002</v>
+        <v>0.3262</v>
       </c>
       <c r="D4" s="1">
-        <v>0.74360000000000004</v>
+        <v>0.0897</v>
       </c>
       <c r="E4" s="1">
-        <v>0.81599999999999995</v>
+        <v>0.7436</v>
       </c>
       <c r="F4" s="1">
-        <v>0.78239999999999998</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G4" s="1">
-        <v>0.68410000000000004</v>
+        <v>0.7824</v>
       </c>
       <c r="H4" s="1">
-        <v>0.42859999999999998</v>
+        <v>0.6841</v>
       </c>
       <c r="I4" s="1">
-        <v>0.47220000000000001</v>
+        <v>0.4286</v>
       </c>
       <c r="J4" s="1">
-        <v>0.72729999999999995</v>
+        <v>0.4722</v>
       </c>
       <c r="K4" s="1">
-        <v>0.42859999999999998</v>
+        <v>0.7272999999999999</v>
       </c>
       <c r="L4" s="1">
-        <v>0.51280000000000003</v>
+        <v>0.4286</v>
       </c>
       <c r="M4" s="1">
-        <v>0.57769999999999999</v>
+        <v>0.5128</v>
       </c>
       <c r="N4" s="1">
-        <v>0.16639999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.5372</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.2085</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>5.1200000000000002E-2</v>
+        <v>0.0512</v>
       </c>
       <c r="C5" s="1">
-        <v>1.8700000000000001E-2</v>
+        <v>0.0187</v>
       </c>
       <c r="D5" s="1">
-        <v>0.27960000000000002</v>
+        <v>0.0149</v>
       </c>
       <c r="E5" s="1">
-        <v>0.65249999999999997</v>
+        <v>0.2796</v>
       </c>
       <c r="F5" s="1">
-        <v>0.70240000000000002</v>
+        <v>0.6525</v>
       </c>
       <c r="G5" s="1">
-        <v>0.34420000000000001</v>
+        <v>0.7024</v>
       </c>
       <c r="H5" s="1">
-        <v>5.4100000000000002E-2</v>
+        <v>0.3442</v>
       </c>
       <c r="I5" s="1">
-        <v>0.1119</v>
+        <v>0.0556</v>
       </c>
       <c r="J5" s="1">
-        <v>0.24390000000000001</v>
+        <v>0.1124</v>
       </c>
       <c r="K5" s="1">
-        <v>0.1111</v>
+        <v>0.1626</v>
       </c>
       <c r="L5" s="1">
-        <v>0.1888</v>
+        <v>0.1167</v>
       </c>
       <c r="M5" s="1">
-        <v>0.25080000000000002</v>
+        <v>0.1759</v>
       </c>
       <c r="N5" s="1">
-        <v>0.22359999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.2239</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.2244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>0.54549999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="1">
-        <v>0.6825</v>
+        <v>0.6923</v>
       </c>
       <c r="D6" s="1">
-        <v>0.62860000000000005</v>
+        <v>0.1987</v>
       </c>
       <c r="E6" s="1">
-        <v>0.87739999999999996</v>
+        <v>0.6562</v>
       </c>
       <c r="F6" s="1">
-        <v>8.7499999999999994E-2</v>
+        <v>0.9024</v>
       </c>
       <c r="G6" s="1">
-        <v>9.8100000000000007E-2</v>
+        <v>0.07969999999999999</v>
       </c>
       <c r="H6" s="1">
-        <v>0.54549999999999998</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="I6" s="1">
-        <v>0.74070000000000003</v>
+        <v>0.5455</v>
       </c>
       <c r="J6" s="1">
-        <v>0.63160000000000005</v>
+        <v>0.7635999999999999</v>
       </c>
       <c r="K6" s="1">
-        <v>0.57140000000000002</v>
+        <v>0.6</v>
       </c>
       <c r="L6" s="1">
-        <v>0.5</v>
+        <v>0.4667</v>
       </c>
       <c r="M6" s="1">
-        <v>0.53720000000000001</v>
+        <v>0.5085</v>
       </c>
       <c r="N6" s="1">
-        <v>0.23219999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.5007</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>0.46150000000000002</v>
+        <v>0.4615</v>
       </c>
       <c r="C7" s="1">
         <v>0.4632</v>
       </c>
       <c r="D7" s="1">
-        <v>8.5699999999999998E-2</v>
+        <v>0.1473</v>
       </c>
       <c r="E7" s="1">
+        <v>0.0857</v>
+      </c>
+      <c r="F7" s="1">
         <v>0.1714</v>
       </c>
-      <c r="F7" s="1">
-        <v>8.5000000000000006E-3</v>
-      </c>
       <c r="G7" s="1">
+        <v>0.008500000000000001</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.1525</v>
       </c>
-      <c r="H7" s="1">
-        <v>0.66669999999999996</v>
-      </c>
       <c r="I7" s="1">
-        <v>0.57779999999999998</v>
+        <v>0.6667</v>
       </c>
       <c r="J7" s="1">
-        <v>0.30769999999999997</v>
+        <v>0.5778</v>
       </c>
       <c r="K7" s="1">
-        <v>0.58330000000000004</v>
+        <v>0.3077</v>
       </c>
       <c r="L7" s="1">
-        <v>0.66669999999999996</v>
+        <v>0.5833</v>
       </c>
       <c r="M7" s="1">
-        <v>0.37680000000000002</v>
+        <v>0.6667</v>
       </c>
       <c r="N7" s="1">
-        <v>0.2303</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.3577</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.2294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1">
-        <v>0.51429999999999998</v>
+        <v>0.5333</v>
       </c>
       <c r="C8" s="1">
-        <v>0.68569999999999998</v>
+        <v>0.6575</v>
       </c>
       <c r="D8" s="1">
-        <v>0.6</v>
+        <v>0.3113</v>
       </c>
       <c r="E8" s="1">
-        <v>0.88839999999999997</v>
+        <v>0.5935</v>
       </c>
       <c r="F8" s="1">
-        <v>0.44280000000000003</v>
+        <v>0.8525</v>
       </c>
       <c r="G8" s="1">
-        <v>0.2273</v>
+        <v>0.4522</v>
       </c>
       <c r="H8" s="1">
-        <v>0.66669999999999996</v>
+        <v>0.2524</v>
       </c>
       <c r="I8" s="1">
-        <v>0.8</v>
+        <v>0.5455</v>
       </c>
       <c r="J8" s="1">
-        <v>0.52170000000000005</v>
+        <v>0.7368</v>
       </c>
       <c r="K8" s="1">
+        <v>0.6667</v>
+      </c>
+      <c r="L8" s="1">
         <v>0.5</v>
       </c>
-      <c r="L8" s="1">
-        <v>0.48280000000000001</v>
-      </c>
       <c r="M8" s="1">
-        <v>0.57540000000000002</v>
+        <v>0.5424</v>
       </c>
       <c r="N8" s="1">
-        <v>0.17299999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.5537</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.1611</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>0.48080000000000001</v>
+        <v>0.4706</v>
       </c>
       <c r="C9" s="1">
-        <v>0.70830000000000004</v>
+        <v>0.7297</v>
       </c>
       <c r="D9" s="1">
-        <v>0.7258</v>
+        <v>0.3935</v>
       </c>
       <c r="E9" s="1">
-        <v>0.9728</v>
+        <v>0.7435</v>
       </c>
       <c r="F9" s="1">
-        <v>0.74</v>
+        <v>0.9801</v>
       </c>
       <c r="G9" s="1">
-        <v>0.6381</v>
+        <v>0.7337</v>
       </c>
       <c r="H9" s="1">
+        <v>0.6389</v>
+      </c>
+      <c r="I9" s="1">
         <v>0.4</v>
       </c>
-      <c r="I9" s="1">
-        <v>0.47370000000000001</v>
-      </c>
       <c r="J9" s="1">
-        <v>0.75860000000000005</v>
+        <v>0.4935</v>
       </c>
       <c r="K9" s="1">
-        <v>0.64859999999999995</v>
+        <v>0.7097</v>
       </c>
       <c r="L9" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.6316000000000001</v>
       </c>
       <c r="M9" s="1">
-        <v>0.64610000000000001</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="N9" s="1">
-        <v>0.15479999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.6237</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.1633</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
-        <v>0.4819</v>
+        <v>0.5714</v>
       </c>
       <c r="C10" s="1">
-        <v>0.57340000000000002</v>
+        <v>0.5921</v>
       </c>
       <c r="D10" s="1">
-        <v>0.61250000000000004</v>
+        <v>0.1722</v>
       </c>
       <c r="E10" s="1">
-        <v>0.81769999999999998</v>
+        <v>0.5472</v>
       </c>
       <c r="F10" s="1">
-        <v>0.3715</v>
+        <v>0.8089</v>
       </c>
       <c r="G10" s="1">
-        <v>0.32679999999999998</v>
+        <v>0.4266</v>
       </c>
       <c r="H10" s="1">
-        <v>0.61539999999999995</v>
+        <v>0.3239</v>
       </c>
       <c r="I10" s="1">
+        <v>0.6667</v>
+      </c>
+      <c r="J10" s="1">
         <v>0.6452</v>
       </c>
-      <c r="J10" s="1">
-        <v>0.53849999999999998</v>
-      </c>
       <c r="K10" s="1">
-        <v>0.51160000000000005</v>
+        <v>0.7272999999999999</v>
       </c>
       <c r="L10" s="1">
-        <v>0.55069999999999997</v>
+        <v>0.4865</v>
       </c>
       <c r="M10" s="1">
-        <v>0.54959999999999998</v>
+        <v>0.5517</v>
       </c>
       <c r="N10" s="1">
-        <v>0.127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.5433</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.1673</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1">
-        <v>0.53849999999999998</v>
+        <v>0.475</v>
       </c>
       <c r="C11" s="1">
-        <v>0.6351</v>
+        <v>0.6531</v>
       </c>
       <c r="D11" s="1">
-        <v>0.55559999999999998</v>
+        <v>0.3396</v>
       </c>
       <c r="E11" s="1">
-        <v>0.80259999999999998</v>
+        <v>0.5995</v>
       </c>
       <c r="F11" s="1">
-        <v>0.45679999999999998</v>
+        <v>0.8061</v>
       </c>
       <c r="G11" s="1">
-        <v>0.25659999999999999</v>
+        <v>0.4241</v>
       </c>
       <c r="H11" s="1">
-        <v>0.54549999999999998</v>
+        <v>0.2266</v>
       </c>
       <c r="I11" s="1">
+        <v>0.6667</v>
+      </c>
+      <c r="J11" s="1">
         <v>0.7</v>
       </c>
-      <c r="J11" s="1">
-        <v>0.59260000000000002</v>
-      </c>
       <c r="K11" s="1">
-        <v>0.57140000000000002</v>
+        <v>0.6087</v>
       </c>
       <c r="L11" s="1">
-        <v>0.56669999999999998</v>
+        <v>0.5161</v>
       </c>
       <c r="M11" s="1">
-        <v>0.56559999999999999</v>
+        <v>0.5424</v>
       </c>
       <c r="N11" s="1">
-        <v>0.13089999999999999</v>
+        <v>0.5465</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0.1553</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:N2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="O1:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Prepare for release (#471)
* Bump version: 0.5.2.dev0 → 0.5.2.dev1

* prepare for release
</commit_message>
<xml_diff>
--- a/benchmark/leaderboard.xlsx
+++ b/benchmark/leaderboard.xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="v0.5.1-Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="v0.5.1-F1-Scores" sheetId="2" r:id="rId2"/>
+    <sheet name="0.5.2-Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="0.5.2-F1-Scores" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>aer</t>
   </si>
@@ -23,16 +23,19 @@
     <t>lstm_dynamic_threshold</t>
   </si>
   <si>
+    <t>matrixprofile</t>
+  </si>
+  <si>
     <t>lstm_autoencoder</t>
   </si>
   <si>
+    <t>arima</t>
+  </si>
+  <si>
+    <t>tadgan</t>
+  </si>
+  <si>
     <t>vae</t>
-  </si>
-  <si>
-    <t>tadgan</t>
-  </si>
-  <si>
-    <t>arima</t>
   </si>
   <si>
     <t>dense_autoencoder</t>
@@ -465,7 +468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -475,24 +478,24 @@
     <col min="2" max="2" width="8.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -500,13 +503,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
-        <v>2231</v>
+        <v>2195</v>
       </c>
       <c r="D2" s="1">
-        <v>0.704</v>
+        <v>0.7169</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -517,13 +520,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>2084</v>
+        <v>2085</v>
       </c>
       <c r="D3" s="1">
-        <v>0.6237</v>
+        <v>0.6357</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -534,16 +537,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>1641</v>
+        <v>2456</v>
       </c>
       <c r="D4" s="1">
-        <v>0.5537</v>
+        <v>0.61</v>
       </c>
       <c r="E4" s="1">
-        <v>0.0003</v>
+        <v>0.0809</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -551,47 +554,47 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>1655</v>
+        <v>1582</v>
       </c>
       <c r="D5" s="1">
-        <v>0.5465</v>
+        <v>0.5574</v>
       </c>
       <c r="E5" s="1">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>7</v>
-      </c>
       <c r="C6" s="1">
-        <v>1861</v>
+        <v>1930</v>
       </c>
       <c r="D6" s="1">
-        <v>0.5433</v>
+        <v>0.5372</v>
       </c>
       <c r="E6" s="1">
-        <v>0.0016</v>
+        <v>0.1425</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="1">
+        <v>7</v>
+      </c>
       <c r="C7" s="1">
-        <v>1930</v>
+        <v>1890</v>
       </c>
       <c r="D7" s="1">
-        <v>0.5372</v>
+        <v>0.5259</v>
       </c>
       <c r="E7" s="1">
-        <v>0.1444</v>
+        <v>0.0016</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -599,13 +602,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>984</v>
+        <v>1634</v>
       </c>
       <c r="D8" s="1">
-        <v>0.5007</v>
+        <v>0.521</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -619,13 +622,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>793</v>
+        <v>965</v>
       </c>
       <c r="D9" s="1">
-        <v>0.3577</v>
+        <v>0.5059</v>
       </c>
       <c r="E9" s="1">
-        <v>0.0296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -633,15 +636,32 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>793</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.3577</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.0296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
         <v>0</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>20912</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>0.2239</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>0</v>
       </c>
     </row>
@@ -652,7 +672,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -677,72 +697,72 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -752,51 +772,51 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>0.5753</v>
+        <v>0.5867</v>
       </c>
       <c r="C3" s="1">
-        <v>0.8031</v>
+        <v>0.7752</v>
       </c>
       <c r="D3" s="1">
-        <v>0.4824</v>
+        <v>0.4738</v>
       </c>
       <c r="E3" s="1">
-        <v>0.7988</v>
+        <v>0.7801</v>
       </c>
       <c r="F3" s="1">
         <v>0.9875</v>
       </c>
       <c r="G3" s="1">
-        <v>0.8977000000000001</v>
+        <v>0.8689</v>
       </c>
       <c r="H3" s="1">
-        <v>0.7125</v>
+        <v>0.6862</v>
       </c>
       <c r="I3" s="1">
-        <v>0.5</v>
+        <v>0.7692</v>
       </c>
       <c r="J3" s="1">
         <v>0.75</v>
       </c>
       <c r="K3" s="1">
-        <v>0.6667</v>
+        <v>0.7333</v>
       </c>
       <c r="L3" s="1">
-        <v>0.7027</v>
+        <v>0.6111</v>
       </c>
       <c r="M3" s="1">
-        <v>0.5714</v>
+        <v>0.5806</v>
       </c>
       <c r="N3" s="1">
-        <v>0.704</v>
+        <v>0.7169</v>
       </c>
       <c r="O3" s="1">
-        <v>0.1486</v>
+        <v>0.1337</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>0.4348</v>
@@ -843,7 +863,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>0.0512</v>
@@ -890,54 +910,54 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>0.5</v>
+        <v>0.5373</v>
       </c>
       <c r="C6" s="1">
-        <v>0.6923</v>
+        <v>0.6405999999999999</v>
       </c>
       <c r="D6" s="1">
-        <v>0.1987</v>
+        <v>0.202</v>
       </c>
       <c r="E6" s="1">
-        <v>0.6562</v>
+        <v>0.6398</v>
       </c>
       <c r="F6" s="1">
-        <v>0.9024</v>
+        <v>0.8853</v>
       </c>
       <c r="G6" s="1">
-        <v>0.07969999999999999</v>
+        <v>0.07770000000000001</v>
       </c>
       <c r="H6" s="1">
-        <v>0.09429999999999999</v>
+        <v>0.1024</v>
       </c>
       <c r="I6" s="1">
         <v>0.5455</v>
       </c>
       <c r="J6" s="1">
-        <v>0.7635999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="K6" s="1">
-        <v>0.6</v>
+        <v>0.6316000000000001</v>
       </c>
       <c r="L6" s="1">
-        <v>0.4667</v>
+        <v>0.5</v>
       </c>
       <c r="M6" s="1">
         <v>0.5085</v>
       </c>
       <c r="N6" s="1">
-        <v>0.5007</v>
+        <v>0.5059</v>
       </c>
       <c r="O6" s="1">
-        <v>0.248</v>
+        <v>0.2455</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>0.4615</v>
@@ -984,49 +1004,49 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
+        <v>0.4789</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.6619</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.3316</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.6195000000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.8741</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.4603</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.2271</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.6667</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.6153999999999999</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.4706</v>
+      </c>
+      <c r="M8" s="1">
         <v>0.5333</v>
       </c>
-      <c r="C8" s="1">
-        <v>0.6575</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.3113</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.5935</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.8525</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.4522</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.2524</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.5455</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0.7368</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.6667</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0.5424</v>
-      </c>
       <c r="N8" s="1">
-        <v>0.5537</v>
+        <v>0.5574</v>
       </c>
       <c r="O8" s="1">
-        <v>0.1611</v>
+        <v>0.1711</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1034,25 +1054,25 @@
         <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>0.4706</v>
+        <v>0.4854</v>
       </c>
       <c r="C9" s="1">
-        <v>0.7297</v>
+        <v>0.7075</v>
       </c>
       <c r="D9" s="1">
-        <v>0.3935</v>
+        <v>0.4169</v>
       </c>
       <c r="E9" s="1">
-        <v>0.7435</v>
+        <v>0.7244</v>
       </c>
       <c r="F9" s="1">
-        <v>0.9801</v>
+        <v>0.9875</v>
       </c>
       <c r="G9" s="1">
-        <v>0.7337</v>
+        <v>0.7437</v>
       </c>
       <c r="H9" s="1">
-        <v>0.6389</v>
+        <v>0.6442</v>
       </c>
       <c r="I9" s="1">
         <v>0.4</v>
@@ -1061,113 +1081,160 @@
         <v>0.4935</v>
       </c>
       <c r="K9" s="1">
-        <v>0.7097</v>
+        <v>0.7586000000000001</v>
       </c>
       <c r="L9" s="1">
-        <v>0.6316000000000001</v>
+        <v>0.6667</v>
       </c>
       <c r="M9" s="1">
-        <v>0.5600000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="N9" s="1">
-        <v>0.6237</v>
+        <v>0.6357</v>
       </c>
       <c r="O9" s="1">
-        <v>0.1633</v>
+        <v>0.1613</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1">
+        <v>0.4737</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.4228</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.4153</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.5073</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.8975</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.793</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.8250999999999999</v>
+      </c>
+      <c r="I10" s="1">
         <v>0.5714</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.5921</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.1722</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.5472</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.8089</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.4266</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0.3239</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0.6667</v>
-      </c>
       <c r="J10" s="1">
-        <v>0.6452</v>
+        <v>0.44</v>
       </c>
       <c r="K10" s="1">
-        <v>0.7272999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="L10" s="1">
-        <v>0.4865</v>
+        <v>0.3529</v>
       </c>
       <c r="M10" s="1">
-        <v>0.5517</v>
+        <v>0.8214</v>
       </c>
       <c r="N10" s="1">
-        <v>0.5433</v>
+        <v>0.61</v>
       </c>
       <c r="O10" s="1">
-        <v>0.1673</v>
+        <v>0.1919</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1">
-        <v>0.475</v>
+        <v>0.5679</v>
       </c>
       <c r="C11" s="1">
-        <v>0.6531</v>
+        <v>0.5897</v>
       </c>
       <c r="D11" s="1">
-        <v>0.3396</v>
+        <v>0.1728</v>
       </c>
       <c r="E11" s="1">
-        <v>0.5995</v>
+        <v>0.5517</v>
       </c>
       <c r="F11" s="1">
-        <v>0.8061</v>
+        <v>0.8056</v>
       </c>
       <c r="G11" s="1">
-        <v>0.4241</v>
+        <v>0.408</v>
       </c>
       <c r="H11" s="1">
-        <v>0.2266</v>
+        <v>0.3211</v>
       </c>
       <c r="I11" s="1">
-        <v>0.6667</v>
+        <v>0.5714</v>
       </c>
       <c r="J11" s="1">
-        <v>0.7</v>
+        <v>0.6032</v>
       </c>
       <c r="K11" s="1">
-        <v>0.6087</v>
+        <v>0.5833</v>
       </c>
       <c r="L11" s="1">
-        <v>0.5161</v>
+        <v>0.5294</v>
       </c>
       <c r="M11" s="1">
-        <v>0.5424</v>
+        <v>0.6061</v>
       </c>
       <c r="N11" s="1">
-        <v>0.5465</v>
+        <v>0.5259</v>
       </c>
       <c r="O11" s="1">
-        <v>0.1553</v>
+        <v>0.1536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.4865</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.649</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.3393</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.5558999999999999</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.8174</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.4149</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.2364</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.4615</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.7368</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.5385</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.4828</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.5333</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.521</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.1538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Release notes for v0.6.0 (#513)
* add release notes

* update release notes

* prepare for release
</commit_message>
<xml_diff>
--- a/benchmark/leaderboard.xlsx
+++ b/benchmark/leaderboard.xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="0.5.2-Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="0.5.2-F1-Scores" sheetId="2" r:id="rId2"/>
+    <sheet name="0.6.0-Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="0.6.0-F1-Scores" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>aer</t>
   </si>
@@ -29,13 +29,16 @@
     <t>arima</t>
   </si>
   <si>
+    <t>vae</t>
+  </si>
+  <si>
+    <t>tadgan</t>
+  </si>
+  <si>
+    <t>lnn</t>
+  </si>
+  <si>
     <t>matrixprofile</t>
-  </si>
-  <si>
-    <t>tadgan</t>
-  </si>
-  <si>
-    <t>vae</t>
   </si>
   <si>
     <t>dense_autoencoder</t>
@@ -468,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -483,19 +486,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -503,13 +506,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
-        <v>2195</v>
+        <v>2244</v>
       </c>
       <c r="D2" s="1">
-        <v>0.7169</v>
+        <v>0.7295</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -523,10 +526,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>2085</v>
+        <v>2087</v>
       </c>
       <c r="D3" s="1">
-        <v>0.6357</v>
+        <v>0.6278</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -537,13 +540,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>1582</v>
+        <v>1617</v>
       </c>
       <c r="D4" s="1">
-        <v>0.5574</v>
+        <v>0.5486</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -554,13 +557,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>1930</v>
+        <v>2135</v>
       </c>
       <c r="D5" s="1">
-        <v>0.5372</v>
+        <v>0.5463</v>
       </c>
       <c r="E5" s="1">
-        <v>0.1425</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -571,10 +574,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>6203</v>
+        <v>1674</v>
       </c>
       <c r="D6" s="1">
-        <v>0.5268</v>
+        <v>0.5375</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -588,10 +591,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>1890</v>
+        <v>1816</v>
       </c>
       <c r="D7" s="1">
-        <v>0.5259</v>
+        <v>0.536</v>
       </c>
       <c r="E7" s="1">
         <v>0.0016</v>
@@ -602,13 +605,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>1634</v>
+        <v>1487</v>
       </c>
       <c r="D8" s="1">
-        <v>0.521</v>
+        <v>0.5351</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -619,13 +622,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
-        <v>965</v>
+        <v>6203</v>
       </c>
       <c r="D9" s="1">
-        <v>0.5059</v>
+        <v>0.5268</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -639,13 +642,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="1">
-        <v>793</v>
+        <v>964</v>
       </c>
       <c r="D10" s="1">
-        <v>0.3577</v>
+        <v>0.514</v>
       </c>
       <c r="E10" s="1">
-        <v>0.0296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -653,15 +656,32 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>793</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.3577</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.0296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
         <v>0</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>20912</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>0.2239</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>0</v>
       </c>
     </row>
@@ -672,7 +692,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -697,72 +717,72 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -775,43 +795,43 @@
         <v>0.5867</v>
       </c>
       <c r="C3" s="1">
-        <v>0.7752</v>
+        <v>0.8189</v>
       </c>
       <c r="D3" s="1">
-        <v>0.4738</v>
+        <v>0.4762</v>
       </c>
       <c r="E3" s="1">
-        <v>0.7801</v>
+        <v>0.7988</v>
       </c>
       <c r="F3" s="1">
         <v>0.9875</v>
       </c>
       <c r="G3" s="1">
-        <v>0.8689</v>
+        <v>0.892</v>
       </c>
       <c r="H3" s="1">
-        <v>0.6862</v>
+        <v>0.7093</v>
       </c>
       <c r="I3" s="1">
-        <v>0.7692</v>
+        <v>0.7143</v>
       </c>
       <c r="J3" s="1">
-        <v>0.75</v>
+        <v>0.7407</v>
       </c>
       <c r="K3" s="1">
-        <v>0.7333</v>
+        <v>0.6897</v>
       </c>
       <c r="L3" s="1">
-        <v>0.6111</v>
+        <v>0.7027</v>
       </c>
       <c r="M3" s="1">
-        <v>0.5806</v>
+        <v>0.6377</v>
       </c>
       <c r="N3" s="1">
-        <v>0.7169</v>
+        <v>0.7295</v>
       </c>
       <c r="O3" s="1">
-        <v>0.1337</v>
+        <v>0.1297</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -819,51 +839,51 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0.4348</v>
+        <v>0.525</v>
       </c>
       <c r="C4" s="1">
-        <v>0.3262</v>
+        <v>0.4115</v>
       </c>
       <c r="D4" s="1">
-        <v>0.0897</v>
+        <v>0.1533</v>
       </c>
       <c r="E4" s="1">
-        <v>0.7436</v>
+        <v>0.7282</v>
       </c>
       <c r="F4" s="1">
-        <v>0.8159999999999999</v>
+        <v>0.8559</v>
       </c>
       <c r="G4" s="1">
-        <v>0.7824</v>
+        <v>0.7972</v>
       </c>
       <c r="H4" s="1">
-        <v>0.6841</v>
+        <v>0.6861</v>
       </c>
       <c r="I4" s="1">
-        <v>0.4286</v>
+        <v>0.3077</v>
       </c>
       <c r="J4" s="1">
-        <v>0.4722</v>
+        <v>0.3824</v>
       </c>
       <c r="K4" s="1">
         <v>0.7272999999999999</v>
       </c>
       <c r="L4" s="1">
-        <v>0.4286</v>
+        <v>0.4667</v>
       </c>
       <c r="M4" s="1">
-        <v>0.5128</v>
+        <v>0.5143</v>
       </c>
       <c r="N4" s="1">
-        <v>0.5372</v>
+        <v>0.5463</v>
       </c>
       <c r="O4" s="1">
-        <v>0.2085</v>
+        <v>0.2058</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>0.0512</v>
@@ -910,54 +930,54 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>0.5373</v>
+        <v>0.5588</v>
       </c>
       <c r="C6" s="1">
-        <v>0.6405999999999999</v>
+        <v>0.6923</v>
       </c>
       <c r="D6" s="1">
-        <v>0.202</v>
+        <v>0.2074</v>
       </c>
       <c r="E6" s="1">
-        <v>0.6398</v>
+        <v>0.6667</v>
       </c>
       <c r="F6" s="1">
-        <v>0.8853</v>
+        <v>0.8924</v>
       </c>
       <c r="G6" s="1">
-        <v>0.07770000000000001</v>
+        <v>0.0697</v>
       </c>
       <c r="H6" s="1">
-        <v>0.1024</v>
+        <v>0.1008</v>
       </c>
       <c r="I6" s="1">
         <v>0.5455</v>
       </c>
       <c r="J6" s="1">
-        <v>0.8</v>
+        <v>0.7635999999999999</v>
       </c>
       <c r="K6" s="1">
-        <v>0.6316000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="L6" s="1">
-        <v>0.5</v>
+        <v>0.5625</v>
       </c>
       <c r="M6" s="1">
         <v>0.5085</v>
       </c>
       <c r="N6" s="1">
-        <v>0.5059</v>
+        <v>0.514</v>
       </c>
       <c r="O6" s="1">
-        <v>0.2455</v>
+        <v>0.2476</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>0.4615</v>
@@ -1004,237 +1024,284 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>0.4789</v>
+        <v>0.5169</v>
       </c>
       <c r="C8" s="1">
-        <v>0.6619</v>
+        <v>0.6182</v>
       </c>
       <c r="D8" s="1">
-        <v>0.3316</v>
+        <v>0.362</v>
       </c>
       <c r="E8" s="1">
-        <v>0.6195000000000001</v>
+        <v>0.6522</v>
       </c>
       <c r="F8" s="1">
-        <v>0.8741</v>
+        <v>0.9381</v>
       </c>
       <c r="G8" s="1">
-        <v>0.4603</v>
+        <v>0.331</v>
       </c>
       <c r="H8" s="1">
-        <v>0.2271</v>
+        <v>0.1908</v>
       </c>
       <c r="I8" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.481</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.7143</v>
+      </c>
+      <c r="L8" s="1">
         <v>0.6667</v>
       </c>
-      <c r="J8" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.6153999999999999</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0.4706</v>
-      </c>
       <c r="M8" s="1">
-        <v>0.5333</v>
+        <v>0.5753</v>
       </c>
       <c r="N8" s="1">
-        <v>0.5574</v>
+        <v>0.5351</v>
       </c>
       <c r="O8" s="1">
-        <v>0.1711</v>
+        <v>0.1943</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1">
-        <v>0.4854</v>
+        <v>0.5455</v>
       </c>
       <c r="C9" s="1">
-        <v>0.7075</v>
+        <v>0.6621</v>
       </c>
       <c r="D9" s="1">
-        <v>0.4169</v>
+        <v>0.327</v>
       </c>
       <c r="E9" s="1">
-        <v>0.7244</v>
+        <v>0.5952</v>
       </c>
       <c r="F9" s="1">
-        <v>0.9875</v>
+        <v>0.8667</v>
       </c>
       <c r="G9" s="1">
-        <v>0.7437</v>
+        <v>0.4659</v>
       </c>
       <c r="H9" s="1">
-        <v>0.6442</v>
+        <v>0.2385</v>
       </c>
       <c r="I9" s="1">
-        <v>0.4</v>
+        <v>0.6667</v>
       </c>
       <c r="J9" s="1">
-        <v>0.4935</v>
+        <v>0.7407</v>
       </c>
       <c r="K9" s="1">
-        <v>0.7586000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="L9" s="1">
-        <v>0.6667</v>
+        <v>0.5</v>
       </c>
       <c r="M9" s="1">
-        <v>0.6</v>
+        <v>0.4746</v>
       </c>
       <c r="N9" s="1">
-        <v>0.6357</v>
+        <v>0.5486</v>
       </c>
       <c r="O9" s="1">
-        <v>0.1613</v>
+        <v>0.1657</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>0.4737</v>
+        <v>0.4706</v>
       </c>
       <c r="C10" s="1">
-        <v>0.4228</v>
+        <v>0.726</v>
       </c>
       <c r="D10" s="1">
-        <v>0.051</v>
+        <v>0.3934</v>
       </c>
       <c r="E10" s="1">
-        <v>0.5073</v>
+        <v>0.7277</v>
       </c>
       <c r="F10" s="1">
-        <v>0.8975</v>
+        <v>0.985</v>
       </c>
       <c r="G10" s="1">
-        <v>0.793</v>
+        <v>0.744</v>
       </c>
       <c r="H10" s="1">
-        <v>0.8250999999999999</v>
+        <v>0.6456</v>
       </c>
       <c r="I10" s="1">
-        <v>0.5714</v>
+        <v>0.4</v>
       </c>
       <c r="J10" s="1">
-        <v>0.44</v>
+        <v>0.4675</v>
       </c>
       <c r="K10" s="1">
-        <v>0.6923</v>
+        <v>0.7857</v>
       </c>
       <c r="L10" s="1">
-        <v>0.3051</v>
+        <v>0.5854</v>
       </c>
       <c r="M10" s="1">
-        <v>0.3429</v>
+        <v>0.6027</v>
       </c>
       <c r="N10" s="1">
-        <v>0.5268</v>
+        <v>0.6278</v>
       </c>
       <c r="O10" s="1">
-        <v>0.2341</v>
+        <v>0.1697</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1">
-        <v>0.5679</v>
+        <v>0.4737</v>
       </c>
       <c r="C11" s="1">
-        <v>0.5897</v>
+        <v>0.4228</v>
       </c>
       <c r="D11" s="1">
-        <v>0.1728</v>
+        <v>0.051</v>
       </c>
       <c r="E11" s="1">
-        <v>0.5517</v>
+        <v>0.5073</v>
       </c>
       <c r="F11" s="1">
-        <v>0.8056</v>
+        <v>0.8975</v>
       </c>
       <c r="G11" s="1">
-        <v>0.408</v>
+        <v>0.793</v>
       </c>
       <c r="H11" s="1">
-        <v>0.3211</v>
+        <v>0.8250999999999999</v>
       </c>
       <c r="I11" s="1">
         <v>0.5714</v>
       </c>
       <c r="J11" s="1">
-        <v>0.6032</v>
+        <v>0.44</v>
       </c>
       <c r="K11" s="1">
-        <v>0.5833</v>
+        <v>0.6923</v>
       </c>
       <c r="L11" s="1">
-        <v>0.5294</v>
+        <v>0.3051</v>
       </c>
       <c r="M11" s="1">
-        <v>0.6061</v>
+        <v>0.3429</v>
       </c>
       <c r="N11" s="1">
-        <v>0.5259</v>
+        <v>0.5268</v>
       </c>
       <c r="O11" s="1">
-        <v>0.1536</v>
+        <v>0.2341</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
-        <v>0.4865</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="C12" s="1">
-        <v>0.649</v>
+        <v>0.6049</v>
       </c>
       <c r="D12" s="1">
-        <v>0.3393</v>
+        <v>0.17</v>
       </c>
       <c r="E12" s="1">
-        <v>0.5558999999999999</v>
+        <v>0.5775</v>
       </c>
       <c r="F12" s="1">
-        <v>0.8174</v>
+        <v>0.8165</v>
       </c>
       <c r="G12" s="1">
-        <v>0.4149</v>
+        <v>0.4164</v>
       </c>
       <c r="H12" s="1">
-        <v>0.2364</v>
+        <v>0.3404</v>
       </c>
       <c r="I12" s="1">
-        <v>0.4615</v>
+        <v>0.5</v>
       </c>
       <c r="J12" s="1">
-        <v>0.7368</v>
+        <v>0.623</v>
       </c>
       <c r="K12" s="1">
-        <v>0.5385</v>
+        <v>0.8182</v>
       </c>
       <c r="L12" s="1">
+        <v>0.4516</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.5538</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.536</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.1752</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.4938</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.6131</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.324</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.5924</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.8034</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.4383</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.2303</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.6667</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.6885</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.5833</v>
+      </c>
+      <c r="L13" s="1">
         <v>0.4828</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M13" s="1">
         <v>0.5333</v>
       </c>
-      <c r="N12" s="1">
-        <v>0.521</v>
-      </c>
-      <c r="O12" s="1">
-        <v>0.1538</v>
+      <c r="N13" s="1">
+        <v>0.5375</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.1516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>